<commit_message>
a correction to makeham_law_mortality.py
</commit_message>
<xml_diff>
--- a/exercisesLifeContingencies/lifeInsurance/Ax_compare_temp_df.xlsx
+++ b/exercisesLifeContingencies/lifeInsurance/Ax_compare_temp_df.xlsx
@@ -1,88 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Dropbox (MagentaKoncept)\PedroCR\PycharmProjects\lifeActuary\exercisesLifeContingencies\lifeInsurance\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F83CB63-269B-4C3F-B672-A504C57EEAA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Ax_compare_temp" sheetId="1" r:id="rId1"/>
+    <sheet name="Ax_compare_temp" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Ax_comm</t>
-  </si>
-  <si>
-    <t>Ax_comm_std_dev</t>
-  </si>
-  <si>
-    <t>Ax_4</t>
-  </si>
-  <si>
-    <t>Ax_4_std_dev</t>
-  </si>
-  <si>
-    <t>Ax_12</t>
-  </si>
-  <si>
-    <t>Ax_12_std_dev</t>
-  </si>
-  <si>
-    <t>Ax_cont</t>
-  </si>
-  <si>
-    <t>Ax_cont_std_dev</t>
-  </si>
-  <si>
-    <t>Ax_comm_4</t>
-  </si>
-  <si>
-    <t>Ax_comm_4_std_dev</t>
-  </si>
-  <si>
-    <t>Ax_comm_12</t>
-  </si>
-  <si>
-    <t>Ax_comm_12_std_dev</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -97,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -421,276 +420,291 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="3.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.265625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_comm</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_comm_std_dev</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_4</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_4_std_dev</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_12</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_12_std_dev</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_cont</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_cont_std_dev</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_comm_4</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_comm_4_std_dev</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_comm_12</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Ax_comm_12_std_dev</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" t="n">
         <v>20</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="n">
         <v>208.75</v>
       </c>
-      <c r="C2">
+      <c r="C2" t="n">
         <v>4031.36</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="n">
         <v>212.6</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="n">
         <v>4106.24</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="n">
         <v>213.47</v>
       </c>
-      <c r="G2">
+      <c r="G2" t="n">
         <v>4122.99</v>
       </c>
-      <c r="H2">
+      <c r="H2" t="n">
         <v>213.9</v>
       </c>
-      <c r="I2">
-        <v>4131.3900000000003</v>
-      </c>
-      <c r="J2">
+      <c r="I2" t="n">
+        <v>4131.39</v>
+      </c>
+      <c r="J2" t="n">
         <v>212.62</v>
       </c>
-      <c r="K2">
-        <v>4106.5600000000004</v>
-      </c>
-      <c r="L2">
+      <c r="K2" t="n">
+        <v>4106.56</v>
+      </c>
+      <c r="L2" t="n">
         <v>213.49</v>
       </c>
-      <c r="M2">
+      <c r="M2" t="n">
         <v>4123.34</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" t="n">
         <v>40</v>
       </c>
-      <c r="B3">
-        <v>573.20000000000005</v>
-      </c>
-      <c r="C3">
+      <c r="B3" t="n">
+        <v>573.2</v>
+      </c>
+      <c r="C3" t="n">
         <v>6584.88</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="n">
         <v>583.65</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="n">
         <v>6705.67</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="n">
         <v>586.02</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="n">
         <v>6732.94</v>
       </c>
-      <c r="H3">
+      <c r="H3" t="n">
         <v>587.21</v>
       </c>
-      <c r="I3">
+      <c r="I3" t="n">
         <v>6746.63</v>
       </c>
-      <c r="J3">
-        <v>583.83000000000004</v>
-      </c>
-      <c r="K3">
+      <c r="J3" t="n">
+        <v>583.83</v>
+      </c>
+      <c r="K3" t="n">
         <v>6707.72</v>
       </c>
-      <c r="L3">
+      <c r="L3" t="n">
         <v>586.22</v>
       </c>
-      <c r="M3">
+      <c r="M3" t="n">
         <v>6735.12</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" t="n">
         <v>60</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="n">
         <v>4252.09</v>
       </c>
-      <c r="C4">
+      <c r="C4" t="n">
         <v>17399.77</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="n">
         <v>4329.26</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="n">
         <v>17717.28</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="n">
         <v>4346.82</v>
       </c>
-      <c r="G4">
-        <v>17789.240000000002</v>
-      </c>
-      <c r="H4">
-        <v>4355.6499999999996</v>
-      </c>
-      <c r="I4">
+      <c r="G4" t="n">
+        <v>17789.24</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4355.65</v>
+      </c>
+      <c r="I4" t="n">
         <v>17825.41</v>
       </c>
-      <c r="J4">
+      <c r="J4" t="n">
         <v>4331.01</v>
       </c>
-      <c r="K4">
+      <c r="K4" t="n">
         <v>17724.45</v>
       </c>
-      <c r="L4">
+      <c r="L4" t="n">
         <v>4348.68</v>
       </c>
-      <c r="M4">
+      <c r="M4" t="n">
         <v>17796.86</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" t="n">
         <v>80</v>
       </c>
-      <c r="B5">
-        <v>33722.160000000003</v>
-      </c>
-      <c r="C5">
+      <c r="B5" t="n">
+        <v>33722.16</v>
+      </c>
+      <c r="C5" t="n">
         <v>38161.74</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="n">
         <v>34340.6</v>
       </c>
-      <c r="E5">
-        <v>38867.339999999997</v>
-      </c>
-      <c r="F5">
+      <c r="E5" t="n">
+        <v>38867.34</v>
+      </c>
+      <c r="F5" t="n">
         <v>34480.26</v>
       </c>
-      <c r="G5">
+      <c r="G5" t="n">
         <v>39025.74</v>
       </c>
-      <c r="H5">
+      <c r="H5" t="n">
         <v>34550.39</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="n">
         <v>39105.17</v>
       </c>
-      <c r="J5">
+      <c r="J5" t="n">
         <v>34348.03</v>
       </c>
-      <c r="K5">
+      <c r="K5" t="n">
         <v>38876.43</v>
       </c>
-      <c r="L5">
-        <v>34488.160000000003</v>
-      </c>
-      <c r="M5">
+      <c r="L5" t="n">
+        <v>34488.16</v>
+      </c>
+      <c r="M5" t="n">
         <v>39035.42</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6">
+    <row r="6">
+      <c r="A6" t="n">
         <v>100</v>
       </c>
-      <c r="B6">
-        <v>86942.080000000002</v>
-      </c>
-      <c r="C6">
-        <v>8748.2000000000007</v>
-      </c>
-      <c r="D6">
+      <c r="B6" t="n">
+        <v>86942.08</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8748.200000000001</v>
+      </c>
+      <c r="D6" t="n">
         <v>88660.7</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>8974.27</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="n">
         <v>89028.66</v>
       </c>
-      <c r="G6">
+      <c r="G6" t="n">
         <v>9014.66</v>
       </c>
-      <c r="H6">
-        <v>89210.68</v>
-      </c>
-      <c r="I6">
+      <c r="H6" t="n">
+        <v>89210.67999999999</v>
+      </c>
+      <c r="I6" t="n">
         <v>9033.49</v>
       </c>
-      <c r="J6">
+      <c r="J6" t="n">
         <v>88555.67</v>
       </c>
-      <c r="K6">
+      <c r="K6" t="n">
         <v>8992.84</v>
       </c>
-      <c r="L6">
+      <c r="L6" t="n">
         <v>88916.95</v>
       </c>
-      <c r="M6">
+      <c r="M6" t="n">
         <v>9034.4</v>
       </c>
     </row>

</xml_diff>